<commit_message>
Adding FL sen and CO gov to two-step forms
</commit_message>
<xml_diff>
--- a/support_files/two_steps.xlsx
+++ b/support_files/two_steps.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="999">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="1081">
   <si>
     <t>Address</t>
   </si>
@@ -3024,6 +3024,252 @@
   </si>
   <si>
     <t>NC </t>
+  </si>
+  <si>
+    <t>FLL000015</t>
+  </si>
+  <si>
+    <t>FLL000034</t>
+  </si>
+  <si>
+    <t>FLL000019</t>
+  </si>
+  <si>
+    <t>FLL000147</t>
+  </si>
+  <si>
+    <t>FLL000017</t>
+  </si>
+  <si>
+    <t>FLL000141</t>
+  </si>
+  <si>
+    <t>FLL000143</t>
+  </si>
+  <si>
+    <t>FLL000002</t>
+  </si>
+  <si>
+    <t>FLL000102</t>
+  </si>
+  <si>
+    <t>FLL000199</t>
+  </si>
+  <si>
+    <t>FLL000022</t>
+  </si>
+  <si>
+    <t>FLL000012</t>
+  </si>
+  <si>
+    <t>FLL000023</t>
+  </si>
+  <si>
+    <t>FLL000086</t>
+  </si>
+  <si>
+    <t>FLL000054</t>
+  </si>
+  <si>
+    <t>FLL000031</t>
+  </si>
+  <si>
+    <t>FLL000190</t>
+  </si>
+  <si>
+    <t>FLL000041</t>
+  </si>
+  <si>
+    <t>FLL000181</t>
+  </si>
+  <si>
+    <t>FLL000064</t>
+  </si>
+  <si>
+    <t>FLL000009</t>
+  </si>
+  <si>
+    <t>FLL000032</t>
+  </si>
+  <si>
+    <t>FLL000026</t>
+  </si>
+  <si>
+    <t>FLL000003</t>
+  </si>
+  <si>
+    <t>FLL000036</t>
+  </si>
+  <si>
+    <t>FLL000027</t>
+  </si>
+  <si>
+    <t>FLL000037</t>
+  </si>
+  <si>
+    <t>FLL000033</t>
+  </si>
+  <si>
+    <t>FLL000025</t>
+  </si>
+  <si>
+    <t>FLL000006</t>
+  </si>
+  <si>
+    <t>FLL000014</t>
+  </si>
+  <si>
+    <t>FLL000016</t>
+  </si>
+  <si>
+    <t>FLL000057</t>
+  </si>
+  <si>
+    <t>FLL000168</t>
+  </si>
+  <si>
+    <t>FLL000010</t>
+  </si>
+  <si>
+    <t>FLL000395</t>
+  </si>
+  <si>
+    <t>FLL000253</t>
+  </si>
+  <si>
+    <t>FLL000170</t>
+  </si>
+  <si>
+    <t>FLL000094</t>
+  </si>
+  <si>
+    <t>FLL000164</t>
+  </si>
+  <si>
+    <t>4300 Legendary Dr Suite 230</t>
+  </si>
+  <si>
+    <t>251 Maitland Ave Suite 304</t>
+  </si>
+  <si>
+    <t>Somewhere</t>
+  </si>
+  <si>
+    <t>101 E Union St Suite 104</t>
+  </si>
+  <si>
+    <t>209 Dunlawton Ave Unit 17</t>
+  </si>
+  <si>
+    <t>2233 Park Ave Suite 303</t>
+  </si>
+  <si>
+    <t>5500 East Highway 100</t>
+  </si>
+  <si>
+    <t>405 Tompkins St</t>
+  </si>
+  <si>
+    <t>5901 SW 16th St</t>
+  </si>
+  <si>
+    <t>1919 Atlantic Blvd</t>
+  </si>
+  <si>
+    <t>1600 Key Deer Blvd</t>
+  </si>
+  <si>
+    <t>1490 W 68th St Suite 201</t>
+  </si>
+  <si>
+    <t>9580 W Calusa Club Dr</t>
+  </si>
+  <si>
+    <t>606 NW 183rd St</t>
+  </si>
+  <si>
+    <t>3050 Biscayne Blvd Suite 600</t>
+  </si>
+  <si>
+    <t>100 NW 1st Ave</t>
+  </si>
+  <si>
+    <t>2600 Hollywood Blvd</t>
+  </si>
+  <si>
+    <t>3500 SW Corporate Pkwy Suite 204</t>
+  </si>
+  <si>
+    <t>2151 NW Sistrunk Blvd</t>
+  </si>
+  <si>
+    <t>2310 1st St Unit 305</t>
+  </si>
+  <si>
+    <t>214 SOB 404 S Monroe St</t>
+  </si>
+  <si>
+    <t>5790 Margate Blvd</t>
+  </si>
+  <si>
+    <t>417 Commercial Ct Suite D</t>
+  </si>
+  <si>
+    <t>508 Lake Ave Unit C</t>
+  </si>
+  <si>
+    <t>1023 Manatee Ave W Suite 201</t>
+  </si>
+  <si>
+    <t>12300 W Forest Hill Blvd Suite 200</t>
+  </si>
+  <si>
+    <t>915 Oakfield Dr Suite D</t>
+  </si>
+  <si>
+    <t>3299 E Tamiami Trl Suite 203</t>
+  </si>
+  <si>
+    <t>3637 4th St N Unit 101</t>
+  </si>
+  <si>
+    <t>205 S Commerce Ave Suite A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26133 US Hwy 19 N Suite 201 </t>
+  </si>
+  <si>
+    <t>209 E Zaragoza St</t>
+  </si>
+  <si>
+    <t>508 W Dr. Martin Luther King Jr. Blvd Suite C</t>
+  </si>
+  <si>
+    <t>5612 Grand Blvd</t>
+  </si>
+  <si>
+    <t>262 Crystal Grove Blvd</t>
+  </si>
+  <si>
+    <t>8910 Astonaut Blvd Suite 210</t>
+  </si>
+  <si>
+    <t>2033 E Edgewood St Suite 101</t>
+  </si>
+  <si>
+    <t>101 N Church St Suite 305</t>
+  </si>
+  <si>
+    <t>1013 E Michigan St</t>
+  </si>
+  <si>
+    <t>511 W South St Suite 204</t>
+  </si>
+  <si>
+    <t>871 S Central Ave Suite C</t>
+  </si>
+  <si>
+    <t>state_tx_gov_greg_abbott</t>
   </si>
 </sst>
 </file>
@@ -3350,13 +3596,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F373"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="A364" sqref="A364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
@@ -9823,182 +10069,838 @@
       </c>
     </row>
     <row r="324" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E324" s="2"/>
-      <c r="F324" s="1"/>
+      <c r="A324" t="s">
+        <v>999</v>
+      </c>
+      <c r="B324" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C324" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D324" t="s">
+        <v>58</v>
+      </c>
+      <c r="E324" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F324" s="1">
+        <v>1111</v>
+      </c>
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E325" s="2"/>
-      <c r="F325" s="1"/>
+      <c r="A325" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B325" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C325" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D325" t="s">
+        <v>58</v>
+      </c>
+      <c r="E325" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F325" s="1">
+        <v>1111</v>
+      </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E326" s="2"/>
-      <c r="F326" s="1"/>
+      <c r="A326" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B326" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C326" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D326" t="s">
+        <v>58</v>
+      </c>
+      <c r="E326" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F326" s="1">
+        <v>1111</v>
+      </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E327" s="2"/>
-      <c r="F327" s="1"/>
+      <c r="A327" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B327" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C327" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D327" t="s">
+        <v>58</v>
+      </c>
+      <c r="E327" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F327" s="1">
+        <v>1111</v>
+      </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E328" s="2"/>
-      <c r="F328" s="1"/>
+      <c r="A328" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B328" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C328" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D328" t="s">
+        <v>58</v>
+      </c>
+      <c r="E328" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F328" s="1">
+        <v>1111</v>
+      </c>
     </row>
     <row r="329" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E329" s="2"/>
-      <c r="F329" s="1"/>
+      <c r="A329" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B329" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C329" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D329" t="s">
+        <v>58</v>
+      </c>
+      <c r="E329" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F329" s="1">
+        <v>1111</v>
+      </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E330" s="2"/>
-      <c r="F330" s="1"/>
+      <c r="A330" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B330" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C330" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D330" t="s">
+        <v>58</v>
+      </c>
+      <c r="E330" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F330" s="1">
+        <v>1111</v>
+      </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E331" s="2"/>
-      <c r="F331" s="1"/>
+      <c r="A331" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B331" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C331" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D331" t="s">
+        <v>58</v>
+      </c>
+      <c r="E331" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F331" s="1">
+        <v>1111</v>
+      </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E332" s="2"/>
-      <c r="F332" s="1"/>
+      <c r="A332" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B332" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C332" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D332" t="s">
+        <v>58</v>
+      </c>
+      <c r="E332" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F332" s="1">
+        <v>1111</v>
+      </c>
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E333" s="2"/>
-      <c r="F333" s="1"/>
+      <c r="A333" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B333" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C333" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D333" t="s">
+        <v>58</v>
+      </c>
+      <c r="E333" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F333" s="1">
+        <v>1111</v>
+      </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E334" s="2"/>
-      <c r="F334" s="1"/>
+      <c r="A334" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B334" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C334" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D334" t="s">
+        <v>58</v>
+      </c>
+      <c r="E334" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F334" s="1">
+        <v>1111</v>
+      </c>
     </row>
     <row r="335" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E335" s="2"/>
-      <c r="F335" s="1"/>
+      <c r="A335" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B335" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C335" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D335" t="s">
+        <v>58</v>
+      </c>
+      <c r="E335" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F335" s="1">
+        <v>1111</v>
+      </c>
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E336" s="2"/>
-      <c r="F336" s="1"/>
-    </row>
-    <row r="337" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E337" s="2"/>
-      <c r="F337" s="1"/>
-    </row>
-    <row r="338" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E338" s="2"/>
-      <c r="F338" s="1"/>
-    </row>
-    <row r="339" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E339" s="2"/>
-      <c r="F339" s="1"/>
-    </row>
-    <row r="340" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E340" s="2"/>
-      <c r="F340" s="1"/>
-    </row>
-    <row r="341" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E341" s="2"/>
-      <c r="F341" s="1"/>
-    </row>
-    <row r="342" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E342" s="2"/>
-      <c r="F342" s="1"/>
-    </row>
-    <row r="343" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E343" s="2"/>
-      <c r="F343" s="1"/>
-    </row>
-    <row r="344" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E344" s="2"/>
-      <c r="F344" s="1"/>
-    </row>
-    <row r="345" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E345" s="2"/>
-      <c r="F345" s="1"/>
-    </row>
-    <row r="346" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E346" s="2"/>
-      <c r="F346" s="1"/>
-    </row>
-    <row r="347" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E347" s="2"/>
-      <c r="F347" s="1"/>
-    </row>
-    <row r="348" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E348" s="2"/>
-      <c r="F348" s="1"/>
-    </row>
-    <row r="349" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E349" s="2"/>
-      <c r="F349" s="1"/>
-    </row>
-    <row r="350" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E350" s="2"/>
-      <c r="F350" s="1"/>
-    </row>
-    <row r="351" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E351" s="2"/>
-      <c r="F351" s="1"/>
-    </row>
-    <row r="352" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E352" s="2"/>
-      <c r="F352" s="1"/>
-    </row>
-    <row r="353" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E353" s="2"/>
-      <c r="F353" s="1"/>
-    </row>
-    <row r="354" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E354" s="2"/>
-      <c r="F354" s="1"/>
-    </row>
-    <row r="355" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E355" s="2"/>
-      <c r="F355" s="1"/>
-    </row>
-    <row r="356" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E356" s="2"/>
-      <c r="F356" s="1"/>
-    </row>
-    <row r="357" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E357" s="2"/>
-      <c r="F357" s="1"/>
-    </row>
-    <row r="358" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E358" s="2"/>
-      <c r="F358" s="1"/>
-    </row>
-    <row r="359" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E359" s="2"/>
-      <c r="F359" s="1"/>
-    </row>
-    <row r="360" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E360" s="2"/>
-      <c r="F360" s="1"/>
-    </row>
-    <row r="361" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E361" s="2"/>
-      <c r="F361" s="1"/>
-    </row>
-    <row r="362" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E362" s="2"/>
-      <c r="F362" s="1"/>
-    </row>
-    <row r="363" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E363" s="2"/>
-      <c r="F363" s="1"/>
-    </row>
-    <row r="364" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E364" s="2"/>
-      <c r="F364" s="1"/>
-    </row>
-    <row r="365" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B336" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C336" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D336" t="s">
+        <v>58</v>
+      </c>
+      <c r="E336" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F336" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B337" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C337" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D337" t="s">
+        <v>58</v>
+      </c>
+      <c r="E337" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F337" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B338" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C338" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D338" t="s">
+        <v>58</v>
+      </c>
+      <c r="E338" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F338" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B339" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C339" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D339" t="s">
+        <v>58</v>
+      </c>
+      <c r="E339" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F339" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B340" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C340" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D340" t="s">
+        <v>58</v>
+      </c>
+      <c r="E340" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F340" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B341" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C341" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D341" t="s">
+        <v>58</v>
+      </c>
+      <c r="E341" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F341" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B342" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C342" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D342" t="s">
+        <v>58</v>
+      </c>
+      <c r="E342" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F342" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B343" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C343" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D343" t="s">
+        <v>58</v>
+      </c>
+      <c r="E343" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F343" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B344" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C344" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D344" t="s">
+        <v>58</v>
+      </c>
+      <c r="E344" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F344" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B345" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C345" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D345" t="s">
+        <v>58</v>
+      </c>
+      <c r="E345" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F345" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B346" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C346" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D346" t="s">
+        <v>58</v>
+      </c>
+      <c r="E346" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F346" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B347" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C347" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D347" t="s">
+        <v>58</v>
+      </c>
+      <c r="E347" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F347" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B348" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C348" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D348" t="s">
+        <v>58</v>
+      </c>
+      <c r="E348" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F348" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B349" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C349" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D349" t="s">
+        <v>58</v>
+      </c>
+      <c r="E349" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F349" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B350" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C350" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D350" t="s">
+        <v>58</v>
+      </c>
+      <c r="E350" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F350" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B351" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C351" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D351" t="s">
+        <v>58</v>
+      </c>
+      <c r="E351" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F351" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B352" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C352" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D352" t="s">
+        <v>58</v>
+      </c>
+      <c r="E352" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F352" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B353" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C353" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D353" t="s">
+        <v>58</v>
+      </c>
+      <c r="E353" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F353" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B354" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C354" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D354" t="s">
+        <v>58</v>
+      </c>
+      <c r="E354" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F354" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B355" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C355" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D355" t="s">
+        <v>58</v>
+      </c>
+      <c r="E355" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F355" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B356" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C356" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D356" t="s">
+        <v>58</v>
+      </c>
+      <c r="E356" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F356" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B357" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C357" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D357" t="s">
+        <v>58</v>
+      </c>
+      <c r="E357" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F357" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B358" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C358" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D358" t="s">
+        <v>58</v>
+      </c>
+      <c r="E358" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F358" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B359" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C359" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D359" t="s">
+        <v>58</v>
+      </c>
+      <c r="E359" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F359" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B360" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C360" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D360" t="s">
+        <v>58</v>
+      </c>
+      <c r="E360" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F360" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B361" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C361" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D361" t="s">
+        <v>58</v>
+      </c>
+      <c r="E361" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F361" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B362" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C362" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D362" t="s">
+        <v>58</v>
+      </c>
+      <c r="E362" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F362" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B363" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C363" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D363" t="s">
+        <v>58</v>
+      </c>
+      <c r="E363" s="2">
+        <v>32541</v>
+      </c>
+      <c r="F363" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B364" t="s">
+        <v>38</v>
+      </c>
+      <c r="C364" t="s">
+        <v>39</v>
+      </c>
+      <c r="D364" t="s">
+        <v>40</v>
+      </c>
+      <c r="E364" s="2">
+        <v>75119</v>
+      </c>
+      <c r="F364" s="1">
+        <v>3624</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E365" s="2"/>
       <c r="F365" s="1"/>
     </row>
-    <row r="366" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E366" s="2"/>
       <c r="F366" s="1"/>
     </row>
-    <row r="367" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E367" s="2"/>
       <c r="F367" s="1"/>
     </row>
-    <row r="368" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E368" s="2"/>
       <c r="F368" s="1"/>
     </row>

</xml_diff>

<commit_message>
Add some forms inside iframes
</commit_message>
<xml_diff>
--- a/support_files/two_steps.xlsx
+++ b/support_files/two_steps.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1874" uniqueCount="1290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2070" uniqueCount="1388">
   <si>
     <t>Address</t>
   </si>
@@ -3897,6 +3897,300 @@
   </si>
   <si>
     <t>214 Test Ave</t>
+  </si>
+  <si>
+    <t>PAL000019</t>
+  </si>
+  <si>
+    <t>215 Test Ave</t>
+  </si>
+  <si>
+    <t>PAL000049</t>
+  </si>
+  <si>
+    <t>PAL000001</t>
+  </si>
+  <si>
+    <t>PAL000048</t>
+  </si>
+  <si>
+    <t>PAL000002</t>
+  </si>
+  <si>
+    <t>PAL000509</t>
+  </si>
+  <si>
+    <t>PAL000003</t>
+  </si>
+  <si>
+    <t>PAL000502</t>
+  </si>
+  <si>
+    <t>PAL000265</t>
+  </si>
+  <si>
+    <t>PAL000004</t>
+  </si>
+  <si>
+    <t>PAL000266</t>
+  </si>
+  <si>
+    <t>PAL000501</t>
+  </si>
+  <si>
+    <t>PAL000005</t>
+  </si>
+  <si>
+    <t>PAL000007</t>
+  </si>
+  <si>
+    <t>PAL000008</t>
+  </si>
+  <si>
+    <t>PAL000009</t>
+  </si>
+  <si>
+    <t>PAL000047</t>
+  </si>
+  <si>
+    <t>PAL000042</t>
+  </si>
+  <si>
+    <t>PAL000013</t>
+  </si>
+  <si>
+    <t>PAL000015</t>
+  </si>
+  <si>
+    <t>PAL000016</t>
+  </si>
+  <si>
+    <t>PAL000050</t>
+  </si>
+  <si>
+    <t>PAL000017</t>
+  </si>
+  <si>
+    <t>PAL000018</t>
+  </si>
+  <si>
+    <t>PAL000496</t>
+  </si>
+  <si>
+    <t>PAL000021</t>
+  </si>
+  <si>
+    <t>PAL000022</t>
+  </si>
+  <si>
+    <t>PAL000224</t>
+  </si>
+  <si>
+    <t>PAL000499</t>
+  </si>
+  <si>
+    <t>PAL000024</t>
+  </si>
+  <si>
+    <t>PAL000026</t>
+  </si>
+  <si>
+    <t>PAL000031</t>
+  </si>
+  <si>
+    <t>PAL000033</t>
+  </si>
+  <si>
+    <t>PAL000035</t>
+  </si>
+  <si>
+    <t>PAL000481</t>
+  </si>
+  <si>
+    <t>PAL000301</t>
+  </si>
+  <si>
+    <t>PAL000137</t>
+  </si>
+  <si>
+    <t>PAL000479</t>
+  </si>
+  <si>
+    <t>PAL000036</t>
+  </si>
+  <si>
+    <t>PAL000494</t>
+  </si>
+  <si>
+    <t>PAL000039</t>
+  </si>
+  <si>
+    <t>PAL000439</t>
+  </si>
+  <si>
+    <t>PAL000040</t>
+  </si>
+  <si>
+    <t>PAL000041</t>
+  </si>
+  <si>
+    <t>PAL000490</t>
+  </si>
+  <si>
+    <t>PAL000043</t>
+  </si>
+  <si>
+    <t>PAL000440</t>
+  </si>
+  <si>
+    <t>PAL000252</t>
+  </si>
+  <si>
+    <t>216 Test Ave</t>
+  </si>
+  <si>
+    <t>217 Test Ave</t>
+  </si>
+  <si>
+    <t>218 Test Ave</t>
+  </si>
+  <si>
+    <t>219 Test Ave</t>
+  </si>
+  <si>
+    <t>220 Test Ave</t>
+  </si>
+  <si>
+    <t>221 Test Ave</t>
+  </si>
+  <si>
+    <t>222 Test Ave</t>
+  </si>
+  <si>
+    <t>223 Test Ave</t>
+  </si>
+  <si>
+    <t>224 Test Ave</t>
+  </si>
+  <si>
+    <t>225 Test Ave</t>
+  </si>
+  <si>
+    <t>226 Test Ave</t>
+  </si>
+  <si>
+    <t>227 Test Ave</t>
+  </si>
+  <si>
+    <t>228 Test Ave</t>
+  </si>
+  <si>
+    <t>229 Test Ave</t>
+  </si>
+  <si>
+    <t>230 Test Ave</t>
+  </si>
+  <si>
+    <t>231 Test Ave</t>
+  </si>
+  <si>
+    <t>232 Test Ave</t>
+  </si>
+  <si>
+    <t>233 Test Ave</t>
+  </si>
+  <si>
+    <t>234 Test Ave</t>
+  </si>
+  <si>
+    <t>235 Test Ave</t>
+  </si>
+  <si>
+    <t>236 Test Ave</t>
+  </si>
+  <si>
+    <t>237 Test Ave</t>
+  </si>
+  <si>
+    <t>238 Test Ave</t>
+  </si>
+  <si>
+    <t>239 Test Ave</t>
+  </si>
+  <si>
+    <t>240 Test Ave</t>
+  </si>
+  <si>
+    <t>241 Test Ave</t>
+  </si>
+  <si>
+    <t>242 Test Ave</t>
+  </si>
+  <si>
+    <t>243 Test Ave</t>
+  </si>
+  <si>
+    <t>244 Test Ave</t>
+  </si>
+  <si>
+    <t>245 Test Ave</t>
+  </si>
+  <si>
+    <t>246 Test Ave</t>
+  </si>
+  <si>
+    <t>247 Test Ave</t>
+  </si>
+  <si>
+    <t>248 Test Ave</t>
+  </si>
+  <si>
+    <t>249 Test Ave</t>
+  </si>
+  <si>
+    <t>250 Test Ave</t>
+  </si>
+  <si>
+    <t>251 Test Ave</t>
+  </si>
+  <si>
+    <t>252 Test Ave</t>
+  </si>
+  <si>
+    <t>253 Test Ave</t>
+  </si>
+  <si>
+    <t>254 Test Ave</t>
+  </si>
+  <si>
+    <t>255 Test Ave</t>
+  </si>
+  <si>
+    <t>256 Test Ave</t>
+  </si>
+  <si>
+    <t>257 Test Ave</t>
+  </si>
+  <si>
+    <t>258 Test Ave</t>
+  </si>
+  <si>
+    <t>259 Test Ave</t>
+  </si>
+  <si>
+    <t>260 Test Ave</t>
+  </si>
+  <si>
+    <t>261 Test Ave</t>
+  </si>
+  <si>
+    <t>262 Test Ave</t>
+  </si>
+  <si>
+    <t>state_nm_gov_susana_martinez</t>
+  </si>
+  <si>
+    <t>263 Test Ave</t>
   </si>
 </sst>
 </file>
@@ -4221,10 +4515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F468"/>
+  <dimension ref="A1:F517"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A345" workbookViewId="0">
-      <selection activeCell="B366" sqref="B366"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E515" sqref="E515"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13595,6 +13889,986 @@
         <v>1111</v>
       </c>
     </row>
+    <row r="469" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B469" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C469" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D469" t="s">
+        <v>64</v>
+      </c>
+      <c r="E469" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F469" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="470" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B470" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C470" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D470" t="s">
+        <v>64</v>
+      </c>
+      <c r="E470" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F470" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="471" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B471" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C471" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D471" t="s">
+        <v>64</v>
+      </c>
+      <c r="E471" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F471" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="472" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B472" t="s">
+        <v>1341</v>
+      </c>
+      <c r="C472" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D472" t="s">
+        <v>64</v>
+      </c>
+      <c r="E472" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F472" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="473" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B473" t="s">
+        <v>1342</v>
+      </c>
+      <c r="C473" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D473" t="s">
+        <v>64</v>
+      </c>
+      <c r="E473" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F473" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="474" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B474" t="s">
+        <v>1343</v>
+      </c>
+      <c r="C474" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D474" t="s">
+        <v>64</v>
+      </c>
+      <c r="E474" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F474" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="475" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B475" t="s">
+        <v>1344</v>
+      </c>
+      <c r="C475" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D475" t="s">
+        <v>64</v>
+      </c>
+      <c r="E475" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F475" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="476" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B476" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C476" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D476" t="s">
+        <v>64</v>
+      </c>
+      <c r="E476" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F476" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="477" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B477" t="s">
+        <v>1346</v>
+      </c>
+      <c r="C477" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D477" t="s">
+        <v>64</v>
+      </c>
+      <c r="E477" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F477" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="478" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B478" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C478" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D478" t="s">
+        <v>64</v>
+      </c>
+      <c r="E478" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F478" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="479" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B479" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C479" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D479" t="s">
+        <v>64</v>
+      </c>
+      <c r="E479" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F479" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="480" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B480" t="s">
+        <v>1349</v>
+      </c>
+      <c r="C480" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D480" t="s">
+        <v>64</v>
+      </c>
+      <c r="E480" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F480" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="481" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B481" t="s">
+        <v>1350</v>
+      </c>
+      <c r="C481" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D481" t="s">
+        <v>64</v>
+      </c>
+      <c r="E481" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F481" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="482" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B482" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C482" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D482" t="s">
+        <v>64</v>
+      </c>
+      <c r="E482" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F482" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="483" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B483" t="s">
+        <v>1352</v>
+      </c>
+      <c r="C483" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D483" t="s">
+        <v>64</v>
+      </c>
+      <c r="E483" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F483" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="484" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B484" t="s">
+        <v>1353</v>
+      </c>
+      <c r="C484" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D484" t="s">
+        <v>64</v>
+      </c>
+      <c r="E484" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F484" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="485" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B485" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C485" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D485" t="s">
+        <v>64</v>
+      </c>
+      <c r="E485" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F485" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="486" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B486" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C486" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D486" t="s">
+        <v>64</v>
+      </c>
+      <c r="E486" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F486" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="487" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B487" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C487" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D487" t="s">
+        <v>64</v>
+      </c>
+      <c r="E487" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F487" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="488" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B488" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C488" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D488" t="s">
+        <v>64</v>
+      </c>
+      <c r="E488" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F488" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="489" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B489" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C489" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D489" t="s">
+        <v>64</v>
+      </c>
+      <c r="E489" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F489" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="490" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A490" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B490" t="s">
+        <v>1359</v>
+      </c>
+      <c r="C490" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D490" t="s">
+        <v>64</v>
+      </c>
+      <c r="E490" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F490" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="491" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B491" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C491" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D491" t="s">
+        <v>64</v>
+      </c>
+      <c r="E491" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F491" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="492" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B492" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C492" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D492" t="s">
+        <v>64</v>
+      </c>
+      <c r="E492" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F492" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="493" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B493" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C493" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D493" t="s">
+        <v>64</v>
+      </c>
+      <c r="E493" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F493" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="494" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A494" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B494" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C494" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D494" t="s">
+        <v>64</v>
+      </c>
+      <c r="E494" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F494" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="495" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B495" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C495" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D495" t="s">
+        <v>64</v>
+      </c>
+      <c r="E495" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F495" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="496" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B496" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C496" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D496" t="s">
+        <v>64</v>
+      </c>
+      <c r="E496" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F496" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="497" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B497" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C497" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D497" t="s">
+        <v>64</v>
+      </c>
+      <c r="E497" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F497" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="498" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B498" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C498" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D498" t="s">
+        <v>64</v>
+      </c>
+      <c r="E498" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F498" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="499" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B499" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C499" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D499" t="s">
+        <v>64</v>
+      </c>
+      <c r="E499" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F499" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="500" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B500" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C500" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D500" t="s">
+        <v>64</v>
+      </c>
+      <c r="E500" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F500" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="501" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A501" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B501" t="s">
+        <v>1370</v>
+      </c>
+      <c r="C501" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D501" t="s">
+        <v>64</v>
+      </c>
+      <c r="E501" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F501" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="502" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A502" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B502" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C502" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D502" t="s">
+        <v>64</v>
+      </c>
+      <c r="E502" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F502" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="503" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B503" t="s">
+        <v>1372</v>
+      </c>
+      <c r="C503" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D503" t="s">
+        <v>64</v>
+      </c>
+      <c r="E503" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F503" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="504" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A504" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B504" t="s">
+        <v>1373</v>
+      </c>
+      <c r="C504" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D504" t="s">
+        <v>64</v>
+      </c>
+      <c r="E504" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F504" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="505" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A505" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B505" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C505" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D505" t="s">
+        <v>64</v>
+      </c>
+      <c r="E505" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F505" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="506" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A506" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B506" t="s">
+        <v>1375</v>
+      </c>
+      <c r="C506" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D506" t="s">
+        <v>64</v>
+      </c>
+      <c r="E506" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F506" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="507" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A507" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B507" t="s">
+        <v>1376</v>
+      </c>
+      <c r="C507" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D507" t="s">
+        <v>64</v>
+      </c>
+      <c r="E507" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F507" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="508" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A508" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B508" t="s">
+        <v>1377</v>
+      </c>
+      <c r="C508" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D508" t="s">
+        <v>64</v>
+      </c>
+      <c r="E508" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F508" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="509" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A509" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B509" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C509" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D509" t="s">
+        <v>64</v>
+      </c>
+      <c r="E509" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F509" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="510" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A510" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B510" t="s">
+        <v>1379</v>
+      </c>
+      <c r="C510" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D510" t="s">
+        <v>64</v>
+      </c>
+      <c r="E510" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F510" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="511" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A511" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B511" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C511" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D511" t="s">
+        <v>64</v>
+      </c>
+      <c r="E511" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F511" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="512" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A512" t="s">
+        <v>1334</v>
+      </c>
+      <c r="B512" t="s">
+        <v>1381</v>
+      </c>
+      <c r="C512" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D512" t="s">
+        <v>64</v>
+      </c>
+      <c r="E512" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F512" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="513" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A513" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B513" t="s">
+        <v>1382</v>
+      </c>
+      <c r="C513" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D513" t="s">
+        <v>64</v>
+      </c>
+      <c r="E513" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F513" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="514" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A514" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B514" t="s">
+        <v>1383</v>
+      </c>
+      <c r="C514" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D514" t="s">
+        <v>64</v>
+      </c>
+      <c r="E514" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F514" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="515" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B515" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C515" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D515" t="s">
+        <v>64</v>
+      </c>
+      <c r="E515" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F515" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="516" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A516" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B516" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C516" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D516" t="s">
+        <v>64</v>
+      </c>
+      <c r="E516" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F516" s="1">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="517" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A517" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B517" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C517" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D517" t="s">
+        <v>416</v>
+      </c>
+      <c r="E517" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F517" s="1">
+        <v>1111</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F373"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Rand Paul has a bad form
</commit_message>
<xml_diff>
--- a/support_files/two_steps.xlsx
+++ b/support_files/two_steps.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2078" uniqueCount="1392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2082" uniqueCount="1394">
   <si>
     <t>Address</t>
   </si>
@@ -4203,6 +4203,12 @@
   </si>
   <si>
     <t>265 Test Ave</t>
+  </si>
+  <si>
+    <t>P000603</t>
+  </si>
+  <si>
+    <t>266 Test Ave</t>
   </si>
 </sst>
 </file>
@@ -4527,10 +4533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F519"/>
+  <dimension ref="A1:F520"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A492" workbookViewId="0">
-      <selection activeCell="F518" sqref="E518:F519"/>
+      <selection activeCell="G512" sqref="G512"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14921,6 +14927,26 @@
         <v>1111</v>
       </c>
     </row>
+    <row r="520" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A520" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B520" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C520" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D520" t="s">
+        <v>117</v>
+      </c>
+      <c r="E520" s="2">
+        <v>11111</v>
+      </c>
+      <c r="F520" s="1">
+        <v>1111</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F373"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add form not in page source
</commit_message>
<xml_diff>
--- a/support_files/two_steps.xlsx
+++ b/support_files/two_steps.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2086" uniqueCount="1397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="1399">
   <si>
     <t>Address</t>
   </si>
@@ -4218,6 +4218,12 @@
   </si>
   <si>
     <t>NAPLES</t>
+  </si>
+  <si>
+    <t>L000174</t>
+  </si>
+  <si>
+    <t>32 MAIN ST</t>
   </si>
 </sst>
 </file>
@@ -4542,10 +4548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F521"/>
+  <dimension ref="A1:F522"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A492" workbookViewId="0">
-      <selection activeCell="B521" sqref="B521:F521"/>
+      <selection activeCell="F523" sqref="F523"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4553,6 +4559,7 @@
     <col min="1" max="1" width="24.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="2"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4569,7 +4576,7 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
@@ -14969,11 +14976,31 @@
       <c r="D521" t="s">
         <v>58</v>
       </c>
-      <c r="E521">
+      <c r="E521" s="2">
         <v>34116</v>
       </c>
       <c r="F521">
         <v>6901</v>
+      </c>
+    </row>
+    <row r="522" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A522" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B522" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C522" t="s">
+        <v>544</v>
+      </c>
+      <c r="D522" t="s">
+        <v>545</v>
+      </c>
+      <c r="E522" s="2">
+        <v>3561</v>
+      </c>
+      <c r="F522">
+        <v>4072</v>
       </c>
     </row>
   </sheetData>

</xml_diff>